<commit_message>
add yaml, new word selection
</commit_message>
<xml_diff>
--- a/filtered_df.xlsx
+++ b/filtered_df.xlsx
@@ -834,7 +834,7 @@
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>팽배</t>
+          <t>파군</t>
         </is>
       </c>
       <c r="B11" t="n">
@@ -845,17 +845,17 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>['ㅍ', 'ㅂ']</t>
+          <t>['ㅍ', 'ㄱ']</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>['ㅐ', 'ㅐ']</t>
+          <t>['ㅏ', 'ㅜ']</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>['ㅇ']</t>
+          <t>['ㄴ']</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -873,7 +873,7 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>난파</t>
+          <t>팽배</t>
         </is>
       </c>
       <c r="B12" t="n">
@@ -884,17 +884,17 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㅍ']</t>
+          <t>['ㅍ', 'ㅂ']</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>['ㅏ', 'ㅏ']</t>
+          <t>['ㅐ', 'ㅐ']</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>['ㄴ']</t>
+          <t>['ㅇ']</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -912,7 +912,7 @@
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>필생</t>
+          <t>난파</t>
         </is>
       </c>
       <c r="B13" t="n">
@@ -923,17 +923,17 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>['ㅍ', 'ㅅ']</t>
+          <t>['ㄴ', 'ㅍ']</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>['ㅣ', 'ㅐ']</t>
+          <t>['ㅏ', 'ㅏ']</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>['ㄹ', 'ㅇ']</t>
+          <t>['ㄴ']</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -942,37 +942,37 @@
         </is>
       </c>
       <c r="H13" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I13" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>매복</t>
+          <t>필생</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C14" t="n">
         <v>2</v>
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>['ㅁ', 'ㅂ']</t>
+          <t>['ㅍ', 'ㅅ']</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>['ㅐ', 'ㅗ']</t>
+          <t>['ㅣ', 'ㅐ']</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>['ㄱ']</t>
+          <t>['ㄹ', 'ㅇ']</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -981,16 +981,16 @@
         </is>
       </c>
       <c r="H14" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I14" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>백태</t>
+          <t>매복</t>
         </is>
       </c>
       <c r="B15" t="n">
@@ -1001,12 +1001,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>['ㅂ', 'ㅌ']</t>
+          <t>['ㅁ', 'ㅂ']</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>['ㅐ', 'ㅐ']</t>
+          <t>['ㅐ', 'ㅗ']</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1020,16 +1020,16 @@
         </is>
       </c>
       <c r="H15" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I15" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>밀사</t>
+          <t>백태</t>
         </is>
       </c>
       <c r="B16" t="n">
@@ -1040,17 +1040,17 @@
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>['ㅁ', 'ㅅ']</t>
+          <t>['ㅂ', 'ㅌ']</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>['ㅣ', 'ㅏ']</t>
+          <t>['ㅐ', 'ㅐ']</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>['ㄹ']</t>
+          <t>['ㄱ']</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1059,16 +1059,16 @@
         </is>
       </c>
       <c r="H16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>무골</t>
+          <t>판본</t>
         </is>
       </c>
       <c r="B17" t="n">
@@ -1079,17 +1079,17 @@
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>['ㅁ', 'ㄱ']</t>
+          <t>['ㅍ', 'ㅂ']</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>['ㅜ', 'ㅗ']</t>
+          <t>['ㅏ', 'ㅗ']</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>['ㄹ']</t>
+          <t>['ㄴ', 'ㄴ']</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1098,16 +1098,16 @@
         </is>
       </c>
       <c r="H17" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I17" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>몰딩</t>
+          <t>밀사</t>
         </is>
       </c>
       <c r="B18" t="n">
@@ -1118,17 +1118,17 @@
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>['ㅁ', 'ㄷ']</t>
+          <t>['ㅁ', 'ㅅ']</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>['ㅗ', 'ㅣ']</t>
+          <t>['ㅣ', 'ㅏ']</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>['ㄹ', 'ㅇ']</t>
+          <t>['ㄹ']</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1146,7 +1146,7 @@
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>비재</t>
+          <t>무골</t>
         </is>
       </c>
       <c r="B19" t="n">
@@ -1157,17 +1157,17 @@
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>['ㅂ', 'ㅈ']</t>
+          <t>['ㅁ', 'ㄱ']</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>['ㅣ', 'ㅐ']</t>
+          <t>['ㅜ', 'ㅗ']</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['ㄹ']</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1185,7 +1185,7 @@
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>새참</t>
+          <t>몰딩</t>
         </is>
       </c>
       <c r="B20" t="n">
@@ -1196,17 +1196,17 @@
       </c>
       <c r="D20" t="inlineStr">
         <is>
-          <t>['ㅅ', 'ㅊ']</t>
+          <t>['ㅁ', 'ㄷ']</t>
         </is>
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>['ㅐ', 'ㅏ']</t>
+          <t>['ㅗ', 'ㅣ']</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>['ㅁ']</t>
+          <t>['ㄹ', 'ㅇ']</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1224,7 +1224,7 @@
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>논개</t>
+          <t>비재</t>
         </is>
       </c>
       <c r="B21" t="n">
@@ -1235,17 +1235,17 @@
       </c>
       <c r="D21" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㄱ']</t>
+          <t>['ㅂ', 'ㅈ']</t>
         </is>
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>['ㅗ', 'ㅐ']</t>
+          <t>['ㅣ', 'ㅐ']</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>['ㄴ']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1254,16 +1254,16 @@
         </is>
       </c>
       <c r="H21" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I21" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>불모</t>
+          <t>새참</t>
         </is>
       </c>
       <c r="B22" t="n">
@@ -1274,17 +1274,17 @@
       </c>
       <c r="D22" t="inlineStr">
         <is>
-          <t>['ㅂ', 'ㅁ']</t>
+          <t>['ㅅ', 'ㅊ']</t>
         </is>
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>['ㅜ', 'ㅗ']</t>
+          <t>['ㅐ', 'ㅏ']</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>['ㄹ']</t>
+          <t>['ㅁ']</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1302,28 +1302,28 @@
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>피폭</t>
+          <t>논개</t>
         </is>
       </c>
       <c r="B23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C23" t="n">
         <v>2</v>
       </c>
       <c r="D23" t="inlineStr">
         <is>
-          <t>['ㅍ', 'ㅍ']</t>
+          <t>['ㄴ', 'ㄱ']</t>
         </is>
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>['ㅣ', 'ㅗ']</t>
+          <t>['ㅗ', 'ㅐ']</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>['ㄱ']</t>
+          <t>['ㄴ']</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1332,7 +1332,7 @@
         </is>
       </c>
       <c r="H23" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I23" t="n">
         <v>0</v>
@@ -1341,28 +1341,28 @@
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>내빈</t>
+          <t>불모</t>
         </is>
       </c>
       <c r="B24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C24" t="n">
         <v>2</v>
       </c>
       <c r="D24" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㅂ']</t>
+          <t>['ㅂ', 'ㅁ']</t>
         </is>
       </c>
       <c r="E24" t="inlineStr">
         <is>
-          <t>['ㅐ', 'ㅣ']</t>
+          <t>['ㅜ', 'ㅗ']</t>
         </is>
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>['ㄴ']</t>
+          <t>['ㄹ']</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1374,13 +1374,13 @@
         <v>0</v>
       </c>
       <c r="I24" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>분개</t>
+          <t>피폭</t>
         </is>
       </c>
       <c r="B25" t="n">
@@ -1391,17 +1391,17 @@
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>['ㅂ', 'ㄱ']</t>
+          <t>['ㅍ', 'ㅍ']</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>['ㅜ', 'ㅐ']</t>
+          <t>['ㅣ', 'ㅗ']</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>['ㄴ']</t>
+          <t>['ㄱ']</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1410,16 +1410,16 @@
         </is>
       </c>
       <c r="H25" t="n">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="I25" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>술책</t>
+          <t>내빈</t>
         </is>
       </c>
       <c r="B26" t="n">
@@ -1430,17 +1430,17 @@
       </c>
       <c r="D26" t="inlineStr">
         <is>
-          <t>['ㅅ', 'ㅊ']</t>
+          <t>['ㄴ', 'ㅂ']</t>
         </is>
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>['ㅜ', 'ㅐ']</t>
+          <t>['ㅐ', 'ㅣ']</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>['ㄹ', 'ㄱ']</t>
+          <t>['ㄴ']</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1458,23 +1458,23 @@
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>시문</t>
+          <t>분개</t>
         </is>
       </c>
       <c r="B27" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C27" t="n">
         <v>2</v>
       </c>
       <c r="D27" t="inlineStr">
         <is>
-          <t>['ㅅ', 'ㅁ']</t>
+          <t>['ㅂ', 'ㄱ']</t>
         </is>
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>['ㅣ', 'ㅜ']</t>
+          <t>['ㅜ', 'ㅐ']</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
@@ -1488,37 +1488,37 @@
         </is>
       </c>
       <c r="H27" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I27" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>뱃심</t>
+          <t>술책</t>
         </is>
       </c>
       <c r="B28" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C28" t="n">
         <v>2</v>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>['ㅂ', 'ㅅ']</t>
+          <t>['ㅅ', 'ㅊ']</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>['ㅐ', 'ㅣ']</t>
+          <t>['ㅜ', 'ㅐ']</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>['ㅅ', 'ㅁ']</t>
+          <t>['ㄹ', 'ㄱ']</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1527,16 +1527,16 @@
         </is>
       </c>
       <c r="H28" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="I28" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>망루</t>
+          <t>시문</t>
         </is>
       </c>
       <c r="B29" t="n">
@@ -1547,17 +1547,17 @@
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>['ㅁ', 'ㄹ']</t>
+          <t>['ㅅ', 'ㅁ']</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>['ㅏ', 'ㅜ']</t>
+          <t>['ㅣ', 'ㅜ']</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>['ㅇ']</t>
+          <t>['ㄴ']</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1566,16 +1566,16 @@
         </is>
       </c>
       <c r="H29" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I29" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>패물</t>
+          <t>뱃심</t>
         </is>
       </c>
       <c r="B30" t="n">
@@ -1586,17 +1586,17 @@
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>['ㅍ', 'ㅁ']</t>
+          <t>['ㅂ', 'ㅅ']</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>['ㅐ', 'ㅜ']</t>
+          <t>['ㅐ', 'ㅣ']</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>['ㄹ']</t>
+          <t>['ㅅ', 'ㅁ']</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1605,37 +1605,37 @@
         </is>
       </c>
       <c r="H30" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="I30" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>닝닝</t>
+          <t>망루</t>
         </is>
       </c>
       <c r="B31" t="n">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C31" t="n">
         <v>2</v>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㄴ']</t>
+          <t>['ㅁ', 'ㄹ']</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
         <is>
-          <t>['ㅣ', 'ㅣ']</t>
+          <t>['ㅏ', 'ㅜ']</t>
         </is>
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>['ㅇ', 'ㅇ']</t>
+          <t>['ㅇ']</t>
         </is>
       </c>
       <c r="G31" t="inlineStr">
@@ -1644,37 +1644,37 @@
         </is>
       </c>
       <c r="H31" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I31" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>수하</t>
+          <t>패물</t>
         </is>
       </c>
       <c r="B32" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C32" t="n">
         <v>2</v>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>['ㅅ', 'ㅎ']</t>
+          <t>['ㅍ', 'ㅁ']</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
         <is>
-          <t>['ㅜ', 'ㅏ']</t>
+          <t>['ㅐ', 'ㅜ']</t>
         </is>
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['ㄹ']</t>
         </is>
       </c>
       <c r="G32" t="inlineStr">
@@ -1686,34 +1686,34 @@
         <v>1</v>
       </c>
       <c r="I32" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>빈축</t>
+          <t>누진</t>
         </is>
       </c>
       <c r="B33" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="C33" t="n">
         <v>2</v>
       </c>
       <c r="D33" t="inlineStr">
         <is>
-          <t>['ㅂ', 'ㅊ']</t>
+          <t>['ㄴ', 'ㅈ']</t>
         </is>
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>['ㅣ', 'ㅜ']</t>
+          <t>['ㅜ', 'ㅣ']</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㄱ']</t>
+          <t>['ㄴ']</t>
         </is>
       </c>
       <c r="G33" t="inlineStr">
@@ -1722,37 +1722,37 @@
         </is>
       </c>
       <c r="H33" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I33" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>박애</t>
+          <t>닝닝</t>
         </is>
       </c>
       <c r="B34" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C34" t="n">
         <v>2</v>
       </c>
       <c r="D34" t="inlineStr">
         <is>
-          <t>['ㅂ', 'ㅇ']</t>
+          <t>['ㄴ', 'ㄴ']</t>
         </is>
       </c>
       <c r="E34" t="inlineStr">
         <is>
-          <t>['ㅏ', 'ㅐ']</t>
+          <t>['ㅣ', 'ㅣ']</t>
         </is>
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>['ㄱ']</t>
+          <t>['ㅇ', 'ㅇ']</t>
         </is>
       </c>
       <c r="G34" t="inlineStr">
@@ -1761,37 +1761,37 @@
         </is>
       </c>
       <c r="H34" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="I34" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>닌자</t>
+          <t>수하</t>
         </is>
       </c>
       <c r="B35" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C35" t="n">
         <v>2</v>
       </c>
       <c r="D35" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㅈ']</t>
+          <t>['ㅅ', 'ㅎ']</t>
         </is>
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>['ㅣ', 'ㅏ']</t>
+          <t>['ㅜ', 'ㅏ']</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>['ㄴ']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G35" t="inlineStr">
@@ -1800,37 +1800,37 @@
         </is>
       </c>
       <c r="H35" t="n">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="I35" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>누룩</t>
+          <t>빈축</t>
         </is>
       </c>
       <c r="B36" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C36" t="n">
         <v>2</v>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㄹ']</t>
+          <t>['ㅂ', 'ㅊ']</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
         <is>
-          <t>['ㅜ', 'ㅜ']</t>
+          <t>['ㅣ', 'ㅜ']</t>
         </is>
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>['ㄱ']</t>
+          <t>['ㄴ', 'ㄱ']</t>
         </is>
       </c>
       <c r="G36" t="inlineStr">
@@ -1842,34 +1842,34 @@
         <v>0</v>
       </c>
       <c r="I36" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>상록</t>
+          <t>복시</t>
         </is>
       </c>
       <c r="B37" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C37" t="n">
         <v>2</v>
       </c>
       <c r="D37" t="inlineStr">
         <is>
-          <t>['ㅅ', 'ㄹ']</t>
+          <t>['ㅂ', 'ㅅ']</t>
         </is>
       </c>
       <c r="E37" t="inlineStr">
         <is>
-          <t>['ㅏ', 'ㅗ']</t>
+          <t>['ㅗ', 'ㅣ']</t>
         </is>
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>['ㅇ', 'ㄱ']</t>
+          <t>['ㄱ']</t>
         </is>
       </c>
       <c r="G37" t="inlineStr">
@@ -1881,34 +1881,34 @@
         <v>0</v>
       </c>
       <c r="I37" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>미비</t>
+          <t>박애</t>
         </is>
       </c>
       <c r="B38" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="C38" t="n">
         <v>2</v>
       </c>
       <c r="D38" t="inlineStr">
         <is>
-          <t>['ㅁ', 'ㅂ']</t>
+          <t>['ㅂ', 'ㅇ']</t>
         </is>
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>['ㅣ', 'ㅣ']</t>
+          <t>['ㅏ', 'ㅐ']</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['ㄱ']</t>
         </is>
       </c>
       <c r="G38" t="inlineStr">
@@ -1917,37 +1917,37 @@
         </is>
       </c>
       <c r="H38" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I38" t="n">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>폭압</t>
+          <t>닌자</t>
         </is>
       </c>
       <c r="B39" t="n">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C39" t="n">
         <v>2</v>
       </c>
       <c r="D39" t="inlineStr">
         <is>
-          <t>['ㅍ', 'ㅇ']</t>
+          <t>['ㄴ', 'ㅈ']</t>
         </is>
       </c>
       <c r="E39" t="inlineStr">
         <is>
-          <t>['ㅗ', 'ㅏ']</t>
+          <t>['ㅣ', 'ㅏ']</t>
         </is>
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>['ㄱ', 'ㅂ']</t>
+          <t>['ㄴ']</t>
         </is>
       </c>
       <c r="G39" t="inlineStr">
@@ -1956,37 +1956,37 @@
         </is>
       </c>
       <c r="H39" t="n">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="I39" t="n">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>발탁</t>
+          <t>누룩</t>
         </is>
       </c>
       <c r="B40" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C40" t="n">
         <v>2</v>
       </c>
       <c r="D40" t="inlineStr">
         <is>
-          <t>['ㅂ', 'ㅌ']</t>
+          <t>['ㄴ', 'ㄹ']</t>
         </is>
       </c>
       <c r="E40" t="inlineStr">
         <is>
-          <t>['ㅏ', 'ㅏ']</t>
+          <t>['ㅜ', 'ㅜ']</t>
         </is>
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>['ㄹ', 'ㄱ']</t>
+          <t>['ㄱ']</t>
         </is>
       </c>
       <c r="G40" t="inlineStr">
@@ -1995,37 +1995,37 @@
         </is>
       </c>
       <c r="H40" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I40" t="n">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>난색</t>
+          <t>상록</t>
         </is>
       </c>
       <c r="B41" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C41" t="n">
         <v>2</v>
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㅅ']</t>
+          <t>['ㅅ', 'ㄹ']</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>['ㅏ', 'ㅐ']</t>
+          <t>['ㅏ', 'ㅗ']</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㄱ']</t>
+          <t>['ㅇ', 'ㄱ']</t>
         </is>
       </c>
       <c r="G41" t="inlineStr">
@@ -2037,34 +2037,34 @@
         <v>0</v>
       </c>
       <c r="I41" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>말미</t>
+          <t>포문</t>
         </is>
       </c>
       <c r="B42" t="n">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="C42" t="n">
         <v>2</v>
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>['ㅁ', 'ㅁ']</t>
+          <t>['ㅍ', 'ㅁ']</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>['ㅏ', 'ㅣ']</t>
+          <t>['ㅗ', 'ㅜ']</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>['ㄹ']</t>
+          <t>['ㄴ']</t>
         </is>
       </c>
       <c r="G42" t="inlineStr">
@@ -2073,32 +2073,32 @@
         </is>
       </c>
       <c r="H42" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I42" t="n">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>노파</t>
+          <t>미비</t>
         </is>
       </c>
       <c r="B43" t="n">
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="C43" t="n">
         <v>2</v>
       </c>
       <c r="D43" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㅍ']</t>
+          <t>['ㅁ', 'ㅂ']</t>
         </is>
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>['ㅗ', 'ㅏ']</t>
+          <t>['ㅣ', 'ㅣ']</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
@@ -2112,37 +2112,37 @@
         </is>
       </c>
       <c r="H43" t="n">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="I43" t="n">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>포부</t>
+          <t>폭압</t>
         </is>
       </c>
       <c r="B44" t="n">
-        <v>29</v>
+        <v>9</v>
       </c>
       <c r="C44" t="n">
         <v>2</v>
       </c>
       <c r="D44" t="inlineStr">
         <is>
-          <t>['ㅍ', 'ㅂ']</t>
+          <t>['ㅍ', 'ㅇ']</t>
         </is>
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>['ㅗ', 'ㅜ']</t>
+          <t>['ㅗ', 'ㅏ']</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['ㄱ', 'ㅂ']</t>
         </is>
       </c>
       <c r="G44" t="inlineStr">
@@ -2151,27 +2151,27 @@
         </is>
       </c>
       <c r="H44" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="I44" t="n">
-        <v>24</v>
+        <v>9</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>소농</t>
+          <t>소조</t>
         </is>
       </c>
       <c r="B45" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C45" t="n">
         <v>2</v>
       </c>
       <c r="D45" t="inlineStr">
         <is>
-          <t>['ㅅ', 'ㄴ']</t>
+          <t>['ㅅ', 'ㅈ']</t>
         </is>
       </c>
       <c r="E45" t="inlineStr">
@@ -2181,7 +2181,7 @@
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>['ㅇ']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G45" t="inlineStr">
@@ -2193,34 +2193,34 @@
         <v>0</v>
       </c>
       <c r="I45" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>봉기</t>
+          <t>내사</t>
         </is>
       </c>
       <c r="B46" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="C46" t="n">
         <v>2</v>
       </c>
       <c r="D46" t="inlineStr">
         <is>
-          <t>['ㅂ', 'ㄱ']</t>
+          <t>['ㄴ', 'ㅅ']</t>
         </is>
       </c>
       <c r="E46" t="inlineStr">
         <is>
-          <t>['ㅗ', 'ㅣ']</t>
+          <t>['ㅐ', 'ㅏ']</t>
         </is>
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>['ㅇ']</t>
+          <t>[]</t>
         </is>
       </c>
       <c r="G46" t="inlineStr">
@@ -2232,34 +2232,34 @@
         <v>0</v>
       </c>
       <c r="I46" t="n">
-        <v>35</v>
+        <v>9</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>판촉</t>
+          <t>발탁</t>
         </is>
       </c>
       <c r="B47" t="n">
-        <v>41</v>
+        <v>10</v>
       </c>
       <c r="C47" t="n">
         <v>2</v>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>['ㅍ', 'ㅊ']</t>
+          <t>['ㅂ', 'ㅌ']</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>['ㅏ', 'ㅗ']</t>
+          <t>['ㅏ', 'ㅏ']</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㄱ']</t>
+          <t>['ㄹ', 'ㄱ']</t>
         </is>
       </c>
       <c r="G47" t="inlineStr">
@@ -2268,37 +2268,37 @@
         </is>
       </c>
       <c r="H47" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="I47" t="n">
-        <v>36</v>
+        <v>9</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>누리</t>
+          <t>상기</t>
         </is>
       </c>
       <c r="B48" t="n">
-        <v>56</v>
+        <v>12</v>
       </c>
       <c r="C48" t="n">
         <v>2</v>
       </c>
       <c r="D48" t="inlineStr">
         <is>
-          <t>['ㄴ', 'ㄹ']</t>
+          <t>['ㅅ', 'ㄱ']</t>
         </is>
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>['ㅜ', 'ㅣ']</t>
+          <t>['ㅏ', 'ㅣ']</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>[]</t>
+          <t>['ㅇ']</t>
         </is>
       </c>
       <c r="G48" t="inlineStr">
@@ -2307,39 +2307,39 @@
         </is>
       </c>
       <c r="H48" t="n">
-        <v>47</v>
+        <v>2</v>
       </c>
       <c r="I48" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>내각</t>
+          <t>난색</t>
         </is>
       </c>
       <c r="B49" t="n">
-        <v>60</v>
+        <v>14</v>
       </c>
       <c r="C49" t="n">
         <v>2</v>
       </c>
       <c r="D49" t="inlineStr">
         <is>
+          <t>['ㄴ', 'ㅅ']</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>['ㅏ', 'ㅐ']</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
           <t>['ㄴ', 'ㄱ']</t>
         </is>
       </c>
-      <c r="E49" t="inlineStr">
-        <is>
-          <t>['ㅐ', 'ㅏ']</t>
-        </is>
-      </c>
-      <c r="F49" t="inlineStr">
-        <is>
-          <t>['ㄱ']</t>
-        </is>
-      </c>
       <c r="G49" t="inlineStr">
         <is>
           <t>Noun</t>
@@ -2349,34 +2349,34 @@
         <v>0</v>
       </c>
       <c r="I49" t="n">
-        <v>60</v>
+        <v>14</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>파문</t>
+          <t>말미</t>
         </is>
       </c>
       <c r="B50" t="n">
-        <v>71</v>
+        <v>14</v>
       </c>
       <c r="C50" t="n">
         <v>2</v>
       </c>
       <c r="D50" t="inlineStr">
         <is>
-          <t>['ㅍ', 'ㅁ']</t>
+          <t>['ㅁ', 'ㅁ']</t>
         </is>
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>['ㅏ', 'ㅜ']</t>
+          <t>['ㅏ', 'ㅣ']</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>['ㄴ']</t>
+          <t>['ㄹ']</t>
         </is>
       </c>
       <c r="G50" t="inlineStr">
@@ -2385,37 +2385,37 @@
         </is>
       </c>
       <c r="H50" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I50" t="n">
-        <v>71</v>
+        <v>13</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>상임</t>
+          <t>녹각</t>
         </is>
       </c>
       <c r="B51" t="n">
-        <v>77</v>
+        <v>14</v>
       </c>
       <c r="C51" t="n">
         <v>2</v>
       </c>
       <c r="D51" t="inlineStr">
         <is>
-          <t>['ㅅ', 'ㅇ']</t>
+          <t>['ㄴ', 'ㄱ']</t>
         </is>
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>['ㅏ', 'ㅣ']</t>
+          <t>['ㅗ', 'ㅏ']</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>['ㅇ', 'ㅁ']</t>
+          <t>['ㄱ', 'ㄱ']</t>
         </is>
       </c>
       <c r="G51" t="inlineStr">
@@ -2427,7 +2427,7 @@
         <v>0</v>
       </c>
       <c r="I51" t="n">
-        <v>77</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>